<commit_message>
Moving to the comparison Gumble Model
</commit_message>
<xml_diff>
--- a/Step2.xlsx
+++ b/Step2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="5_{17E023A8-9766-4E9C-900C-D09D8233477B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6BB6B9FC-45C9-440B-BEFC-1FDEE0843333}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -456,10 +456,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>40909</v>
+        <v>43117</v>
       </c>
       <c r="B4">
-        <v>30.5</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -507,10 +507,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>40909</v>
+        <v>37548</v>
       </c>
       <c r="B7">
-        <v>30.5</v>
+        <v>63</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -587,46 +587,46 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>40909</v>
+        <v>37548</v>
       </c>
       <c r="B2">
-        <v>30.5</v>
+        <v>63</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>40909</v>
+        <v>43123</v>
       </c>
       <c r="B3">
-        <v>30.5</v>
+        <v>65</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>43123</v>
+        <v>38928</v>
       </c>
       <c r="B4">
         <v>65</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>38928</v>
+        <v>43117</v>
       </c>
       <c r="B5">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>